<commit_message>
Customer RestApi 11번까지 구현
</commit_message>
<xml_diff>
--- a/프로젝트 회의록/기능테스트.xlsx
+++ b/프로젝트 회의록/기능테스트.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byh98\Desktop\GitHub\StuppingMall\프로젝트 회의록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF304E56-16A6-42F3-9832-FB31F73073B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC24076-6BFD-4376-B24D-452932D1F099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{E4CF1CAF-4740-494B-8FD6-E9F5FCF1639C}"/>
+    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E4CF1CAF-4740-494B-8FD6-E9F5FCF1639C}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer 기능" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
   <si>
     <t>메인 페이지 접속</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -317,30 +317,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>그래프 아이템 검색</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>비교 페이지 접속</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/graph/index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/graph/items</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>그래프 아이템 확정</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>/graph/item/:id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>로그인 페이지 접속</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -526,6 +506,30 @@
   </si>
   <si>
     <t>페이지, 정렬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comparison/index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comparison/items</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/comparison/item/:id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프론트단에서 처리하도록 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비교 아이템 검색</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비교 아이템 확정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1673,7 +1677,7 @@
   <dimension ref="B1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1683,7 +1687,7 @@
     <col min="5" max="5" width="22.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1702,10 +1706,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -1773,7 +1777,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
@@ -1830,7 +1834,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1855,13 +1859,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>65</v>
+        <v>111</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1872,13 +1876,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>66</v>
+        <v>112</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>58</v>
@@ -1891,30 +1895,32 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>67</v>
+        <v>116</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>68</v>
+        <v>113</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="10">
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1931,7 +1937,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1942,13 +1948,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1959,13 +1965,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1976,13 +1982,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1999,7 +2005,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -2010,18 +2016,18 @@
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -2029,18 +2035,18 @@
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -2048,13 +2054,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -2065,13 +2071,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -2082,13 +2088,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -2099,13 +2105,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -2116,13 +2122,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -2133,13 +2139,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2150,13 +2156,13 @@
         <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -2167,13 +2173,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2190,10 +2196,10 @@
         <v>49</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="6"/>
@@ -2203,13 +2209,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2220,13 +2226,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2237,13 +2243,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2254,16 +2260,16 @@
         <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="6"/>

</xml_diff>

<commit_message>
Customer RestApi 21번까지 구현
</commit_message>
<xml_diff>
--- a/프로젝트 회의록/기능테스트.xlsx
+++ b/프로젝트 회의록/기능테스트.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byh98\Desktop\GitHub\StuppingMall\프로젝트 회의록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC24076-6BFD-4376-B24D-452932D1F099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74CACD-2BF5-498C-B148-0782AFEED3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E4CF1CAF-4740-494B-8FD6-E9F5FCF1639C}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="118">
   <si>
     <t>메인 페이지 접속</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -530,6 +530,10 @@
   </si>
   <si>
     <t>비교 아이템 확정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>key, newPassword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1091,7 +1095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BB52DA5-059C-43C0-AC51-AF7BDF69CA64}">
   <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -1532,7 +1536,7 @@
   <dimension ref="B2:E13"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1676,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C97BF40-7CD3-4EE7-BE1E-9755732F8468}">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2079,7 +2083,9 @@
       <c r="E23" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
     </row>

</xml_diff>

<commit_message>
Customer RestApi 26번까지 구현
</commit_message>
<xml_diff>
--- a/프로젝트 회의록/기능테스트.xlsx
+++ b/프로젝트 회의록/기능테스트.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byh98\Desktop\GitHub\StuppingMall\프로젝트 회의록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D74CACD-2BF5-498C-B148-0782AFEED3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7758AF27-6258-432C-A66E-CCFBE033170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E4CF1CAF-4740-494B-8FD6-E9F5FCF1639C}"/>
   </bookViews>
@@ -381,10 +381,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/customer/recents</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/customer/reports</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -534,6 +530,10 @@
   </si>
   <si>
     <t>key, newPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/customer/recentFinds</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C97BF40-7CD3-4EE7-BE1E-9755732F8468}">
   <dimension ref="B1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1710,10 +1710,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -1781,7 +1781,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
@@ -1838,7 +1838,7 @@
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1869,7 +1869,7 @@
         <v>43</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1880,13 +1880,13 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>58</v>
@@ -1899,18 +1899,18 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -1969,13 +1969,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1986,13 +1986,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -2020,18 +2020,18 @@
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -2039,18 +2039,18 @@
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -2058,13 +2058,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -2075,16 +2075,16 @@
         <v>21</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>72</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
@@ -2151,7 +2151,7 @@
         <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2168,7 +2168,7 @@
         <v>43</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -2179,13 +2179,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2202,10 +2202,10 @@
         <v>49</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="6"/>
@@ -2215,13 +2215,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2232,13 +2232,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2249,13 +2249,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2266,16 +2266,16 @@
         <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="6"/>

</xml_diff>

<commit_message>
customer 기능 1차 완료
</commit_message>
<xml_diff>
--- a/프로젝트 회의록/기능테스트.xlsx
+++ b/프로젝트 회의록/기능테스트.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\byh98\Desktop\GitHub\StuppingMall\프로젝트 회의록\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7758AF27-6258-432C-A66E-CCFBE033170F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C5402D-7026-4C06-8BC5-5810154FF91A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5280" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E4CF1CAF-4740-494B-8FD6-E9F5FCF1639C}"/>
+    <workbookView xWindow="38400" yWindow="5595" windowWidth="28800" windowHeight="15345" activeTab="3" xr2:uid="{E4CF1CAF-4740-494B-8FD6-E9F5FCF1639C}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer 기능" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="123">
   <si>
     <t>메인 페이지 접속</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -273,10 +273,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>구매 요청</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이미지 자세히보기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -534,6 +530,30 @@
   </si>
   <si>
     <t>/customer/recentFinds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELETE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 탈퇴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/customer/balance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품 주문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>money</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1678,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C97BF40-7CD3-4EE7-BE1E-9755732F8468}">
-  <dimension ref="B1:H34"/>
+  <dimension ref="B1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1710,10 +1730,10 @@
         <v>51</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -1772,7 +1792,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>49</v>
@@ -1781,7 +1801,7 @@
         <v>50</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="6"/>
@@ -1791,13 +1811,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -1808,13 +1828,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1825,20 +1845,20 @@
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -1846,13 +1866,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
@@ -1863,13 +1883,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
@@ -1880,16 +1900,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
@@ -1899,18 +1919,18 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
@@ -1918,13 +1938,13 @@
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
@@ -1941,7 +1961,7 @@
         <v>49</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
@@ -1952,13 +1972,13 @@
         <v>14</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1969,13 +1989,13 @@
         <v>15</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1986,13 +2006,13 @@
         <v>16</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -2009,7 +2029,7 @@
         <v>49</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -2020,18 +2040,18 @@
         <v>18</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
@@ -2039,18 +2059,18 @@
         <v>19</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
@@ -2058,13 +2078,13 @@
         <v>20</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -2075,16 +2095,16 @@
         <v>21</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="F23" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="6"/>
@@ -2094,13 +2114,13 @@
         <v>22</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -2111,13 +2131,13 @@
         <v>23</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -2128,13 +2148,13 @@
         <v>24</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -2145,13 +2165,13 @@
         <v>25</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -2162,13 +2182,13 @@
         <v>26</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -2179,13 +2199,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2202,10 +2222,10 @@
         <v>49</v>
       </c>
       <c r="E30" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="6"/>
@@ -2215,13 +2235,13 @@
         <v>29</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2232,13 +2252,13 @@
         <v>30</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>43</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -2249,13 +2269,13 @@
         <v>31</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -2266,19 +2286,66 @@
         <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="10">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="10">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="10">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>